<commit_message>
Now getting the order right even when there's non-detects
</commit_message>
<xml_diff>
--- a/vignettes/OWC_custom_bench.xlsx
+++ b/vignettes/OWC_custom_bench.xlsx
@@ -1037,6 +1037,9 @@
     <t xml:space="preserve">StRegis</t>
   </si>
   <si>
+    <t xml:space="preserve">chm_nm</t>
+  </si>
+  <si>
     <t xml:space="preserve">groupCol</t>
   </si>
   <si>
@@ -1050,9 +1053,6 @@
   </si>
   <si>
     <t xml:space="preserve">chronic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tribromomethane (bromoform)</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -82111,16 +82111,19 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>340</v>
       </c>
       <c r="C1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2">
@@ -82131,13 +82134,16 @@
         <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E2" t="n">
         <v>86.1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3">
@@ -82148,13 +82154,16 @@
         <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E3" t="n">
         <v>3.98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4">
@@ -82165,13 +82174,16 @@
         <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E4" t="n">
         <v>29.6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="5">
@@ -82182,13 +82194,16 @@
         <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E5" t="n">
         <v>803</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6">
@@ -82199,13 +82214,16 @@
         <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E6" t="n">
         <v>79.7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7">
@@ -82216,13 +82234,16 @@
         <v>135</v>
       </c>
       <c r="C7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E7" t="n">
         <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8">
@@ -82233,13 +82254,16 @@
         <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E8" t="n">
         <v>2140</v>
+      </c>
+      <c r="F8" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="9">
@@ -82250,13 +82274,16 @@
         <v>153</v>
       </c>
       <c r="C9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E9" t="n">
         <v>360</v>
+      </c>
+      <c r="F9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10">
@@ -82267,13 +82294,16 @@
         <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E10" t="n">
         <v>14000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11">
@@ -82284,13 +82314,16 @@
         <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D11" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E11" t="n">
         <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12">
@@ -82301,13 +82334,16 @@
         <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E12" t="n">
         <v>98</v>
+      </c>
+      <c r="F12" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13">
@@ -82318,13 +82354,16 @@
         <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E13" t="n">
         <v>0.85</v>
+      </c>
+      <c r="F13" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="14">
@@ -82335,13 +82374,16 @@
         <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D14" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E14" t="n">
         <v>0.05</v>
+      </c>
+      <c r="F14" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="15">
@@ -82352,13 +82394,16 @@
         <v>166</v>
       </c>
       <c r="C15" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D15" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E15" t="n">
         <v>0.17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="16">
@@ -82369,13 +82414,16 @@
         <v>167</v>
       </c>
       <c r="C16" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E16" t="n">
         <v>0.035</v>
+      </c>
+      <c r="F16" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="17">
@@ -82386,13 +82434,16 @@
         <v>178</v>
       </c>
       <c r="C17" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D17" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E17" t="n">
         <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="18">
@@ -82403,13 +82454,16 @@
         <v>130</v>
       </c>
       <c r="C18" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E18" t="n">
         <v>20.7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="19">
@@ -82420,13 +82474,16 @@
         <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D19" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E19" t="n">
         <v>0.014</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="20">
@@ -82437,13 +82494,16 @@
         <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D20" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E20" t="n">
         <v>7.11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21">
@@ -82454,13 +82514,16 @@
         <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D21" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E21" t="n">
         <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22">
@@ -82471,13 +82534,16 @@
         <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D22" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E22" t="n">
         <v>6.3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23">
@@ -82488,13 +82554,16 @@
         <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D23" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E23" t="n">
         <v>10.1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="24">
@@ -82505,13 +82574,16 @@
         <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D24" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E24" t="n">
         <v>220</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="25">
@@ -82522,13 +82594,16 @@
         <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D25" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E25" t="n">
         <v>2.1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="26">
@@ -82539,13 +82614,16 @@
         <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D26" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E26" t="n">
         <v>4.7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="27">
@@ -82556,13 +82634,16 @@
         <v>148</v>
       </c>
       <c r="C27" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D27" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E27" t="n">
         <v>2.6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="28">
@@ -82573,13 +82654,16 @@
         <v>153</v>
       </c>
       <c r="C28" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D28" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E28" t="n">
         <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="29">
@@ -82590,13 +82674,16 @@
         <v>156</v>
       </c>
       <c r="C29" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D29" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E29" t="n">
         <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="30">
@@ -82607,13 +82694,16 @@
         <v>158</v>
       </c>
       <c r="C30" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D30" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E30" t="n">
         <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="31">
@@ -82624,13 +82714,16 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D31" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E31" t="n">
         <v>0.5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="32">
@@ -82641,13 +82734,16 @@
         <v>164</v>
       </c>
       <c r="C32" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D32" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E32" t="n">
         <v>0.04</v>
+      </c>
+      <c r="F32" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="33">
@@ -82658,13 +82754,16 @@
         <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D33" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E33" t="n">
         <v>0.043</v>
+      </c>
+      <c r="F33" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="34">
@@ -82675,13 +82774,16 @@
         <v>167</v>
       </c>
       <c r="C34" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D34" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E34" t="n">
         <v>0.0058</v>
+      </c>
+      <c r="F34" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="35">
@@ -82692,13 +82794,16 @@
         <v>178</v>
       </c>
       <c r="C35" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D35" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E35" t="n">
         <v>6.6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="36">
@@ -82709,13 +82814,16 @@
         <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E36" t="n">
         <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="37">
@@ -82723,16 +82831,19 @@
         <v>29</v>
       </c>
       <c r="B37" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" t="s">
+        <v>343</v>
+      </c>
+      <c r="D37" t="s">
         <v>345</v>
-      </c>
-      <c r="C37" t="s">
-        <v>342</v>
-      </c>
-      <c r="D37" t="s">
-        <v>344</v>
       </c>
       <c r="E37" t="n">
         <v>320</v>
+      </c>
+      <c r="F37" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="38">
@@ -82746,10 +82857,13 @@
         <v>346</v>
       </c>
       <c r="D38" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E38" t="n">
         <v>1518</v>
+      </c>
+      <c r="F38" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="39">
@@ -82763,10 +82877,13 @@
         <v>346</v>
       </c>
       <c r="D39" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E39" t="n">
         <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="40">
@@ -82780,10 +82897,13 @@
         <v>346</v>
       </c>
       <c r="D40" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E40" t="n">
         <v>0.24</v>
+      </c>
+      <c r="F40" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="41">
@@ -82797,10 +82917,13 @@
         <v>346</v>
       </c>
       <c r="D41" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E41" t="n">
         <v>3980</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="42">
@@ -82814,10 +82937,13 @@
         <v>346</v>
       </c>
       <c r="D42" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E42" t="n">
         <v>190</v>
+      </c>
+      <c r="F42" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="43">
@@ -82831,10 +82957,13 @@
         <v>346</v>
       </c>
       <c r="D43" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E43" t="n">
         <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="44">
@@ -82848,10 +82977,13 @@
         <v>346</v>
       </c>
       <c r="D44" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E44" t="n">
         <v>1800</v>
+      </c>
+      <c r="F44" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="45">
@@ -82865,10 +82997,13 @@
         <v>346</v>
       </c>
       <c r="D45" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E45" t="n">
         <v>37</v>
+      </c>
+      <c r="F45" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="46">
@@ -82882,10 +83017,13 @@
         <v>346</v>
       </c>
       <c r="D46" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E46" t="n">
         <v>117000</v>
+      </c>
+      <c r="F46" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="47">
@@ -82899,10 +83037,13 @@
         <v>346</v>
       </c>
       <c r="D47" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E47" t="n">
         <v>830</v>
+      </c>
+      <c r="F47" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="48">
@@ -82916,10 +83057,13 @@
         <v>346</v>
       </c>
       <c r="D48" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E48" t="n">
         <v>3.3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="49">
@@ -82933,10 +83077,13 @@
         <v>346</v>
       </c>
       <c r="D49" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E49" t="n">
         <v>0.02</v>
+      </c>
+      <c r="F49" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="50">
@@ -82950,10 +83097,13 @@
         <v>346</v>
       </c>
       <c r="D50" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E50" t="n">
         <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="51">
@@ -82961,16 +83111,19 @@
         <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>345</v>
+        <v>209</v>
       </c>
       <c r="C51" t="s">
         <v>346</v>
       </c>
       <c r="D51" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E51" t="n">
         <v>2300</v>
+      </c>
+      <c r="F51" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="52">
@@ -82984,10 +83137,13 @@
         <v>346</v>
       </c>
       <c r="D52" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E52" t="n">
         <v>0.86</v>
+      </c>
+      <c r="F52" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="53">
@@ -83001,10 +83157,13 @@
         <v>346</v>
       </c>
       <c r="D53" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E53" t="n">
         <v>0.012</v>
+      </c>
+      <c r="F53" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="54">
@@ -83018,10 +83177,13 @@
         <v>346</v>
       </c>
       <c r="D54" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E54" t="n">
         <v>0.015</v>
+      </c>
+      <c r="F54" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="55">
@@ -83035,10 +83197,13 @@
         <v>346</v>
       </c>
       <c r="D55" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E55" t="n">
         <v>0.04</v>
+      </c>
+      <c r="F55" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="56">
@@ -83052,10 +83217,13 @@
         <v>346</v>
       </c>
       <c r="D56" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E56" t="n">
         <v>1.1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="57">
@@ -83069,10 +83237,13 @@
         <v>346</v>
       </c>
       <c r="D57" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E57" t="n">
         <v>0.4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="58">
@@ -83086,10 +83257,13 @@
         <v>346</v>
       </c>
       <c r="D58" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E58" t="n">
         <v>0.025</v>
+      </c>
+      <c r="F58" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="59">
@@ -83103,10 +83277,13 @@
         <v>346</v>
       </c>
       <c r="D59" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E59" t="n">
         <v>110</v>
+      </c>
+      <c r="F59" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="60">
@@ -83120,10 +83297,13 @@
         <v>346</v>
       </c>
       <c r="D60" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E60" t="n">
         <v>2.1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="61">
@@ -83137,10 +83317,13 @@
         <v>346</v>
       </c>
       <c r="D61" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E61" t="n">
         <v>330</v>
+      </c>
+      <c r="F61" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="62">
@@ -83154,10 +83337,13 @@
         <v>346</v>
       </c>
       <c r="D62" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E62" t="n">
         <v>920</v>
+      </c>
+      <c r="F62" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="63">
@@ -83171,10 +83357,13 @@
         <v>346</v>
       </c>
       <c r="D63" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E63" t="n">
         <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="64">
@@ -83188,10 +83377,13 @@
         <v>346</v>
       </c>
       <c r="D64" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E64" t="n">
         <v>1.8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="65">
@@ -83205,10 +83397,13 @@
         <v>346</v>
       </c>
       <c r="D65" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E65" t="n">
         <v>5</v>
+      </c>
+      <c r="F65" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="66">
@@ -83222,10 +83417,13 @@
         <v>346</v>
       </c>
       <c r="D66" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E66" t="n">
         <v>7.8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="67">
@@ -83239,10 +83437,13 @@
         <v>346</v>
       </c>
       <c r="D67" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E67" t="n">
         <v>0.2</v>
+      </c>
+      <c r="F67" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="68">
@@ -83256,10 +83457,13 @@
         <v>346</v>
       </c>
       <c r="D68" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E68" t="n">
         <v>0.002</v>
+      </c>
+      <c r="F68" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="69">
@@ -83273,10 +83477,13 @@
         <v>346</v>
       </c>
       <c r="D69" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="70">
@@ -83290,10 +83497,13 @@
         <v>346</v>
       </c>
       <c r="D70" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E70" t="n">
         <v>9.4</v>
+      </c>
+      <c r="F70" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="71">
@@ -83301,16 +83511,19 @@
         <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>345</v>
+        <v>209</v>
       </c>
       <c r="C71" t="s">
         <v>346</v>
       </c>
       <c r="D71" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E71" t="n">
         <v>320</v>
+      </c>
+      <c r="F71" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing plot heights based on review comments
</commit_message>
<xml_diff>
--- a/vignettes/OWC_custom_bench.xlsx
+++ b/vignettes/OWC_custom_bench.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="349">
   <si>
     <t xml:space="preserve">SiteID</t>
   </si>
@@ -1055,9 +1055,6 @@
     <t xml:space="preserve">Benzo[a]pyrene</t>
   </si>
   <si>
-    <t xml:space="preserve">1-Naphthalenol, 1-(N-methylcarbamate)</t>
-  </si>
-  <si>
     <t xml:space="preserve">chronic</t>
   </si>
   <si>
@@ -82369,7 +82366,7 @@
         <v>0.85</v>
       </c>
       <c r="F13" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14">
@@ -82463,7 +82460,7 @@
         <v>343</v>
       </c>
       <c r="D18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E18" t="n">
         <v>20.7</v>
@@ -82483,7 +82480,7 @@
         <v>343</v>
       </c>
       <c r="D19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E19" t="n">
         <v>0.014</v>
@@ -82503,7 +82500,7 @@
         <v>343</v>
       </c>
       <c r="D20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E20" t="n">
         <v>7.11</v>
@@ -82523,7 +82520,7 @@
         <v>343</v>
       </c>
       <c r="D21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E21" t="n">
         <v>24</v>
@@ -82543,7 +82540,7 @@
         <v>343</v>
       </c>
       <c r="D22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E22" t="n">
         <v>6.3</v>
@@ -82563,7 +82560,7 @@
         <v>343</v>
       </c>
       <c r="D23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E23" t="n">
         <v>10.1</v>
@@ -82583,7 +82580,7 @@
         <v>343</v>
       </c>
       <c r="D24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E24" t="n">
         <v>220</v>
@@ -82603,7 +82600,7 @@
         <v>343</v>
       </c>
       <c r="D25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E25" t="n">
         <v>2.1</v>
@@ -82623,7 +82620,7 @@
         <v>343</v>
       </c>
       <c r="D26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E26" t="n">
         <v>4.7</v>
@@ -82643,7 +82640,7 @@
         <v>343</v>
       </c>
       <c r="D27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E27" t="n">
         <v>2.6</v>
@@ -82663,7 +82660,7 @@
         <v>343</v>
       </c>
       <c r="D28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E28" t="n">
         <v>60</v>
@@ -82683,7 +82680,7 @@
         <v>343</v>
       </c>
       <c r="D29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E29" t="n">
         <v>100</v>
@@ -82703,7 +82700,7 @@
         <v>343</v>
       </c>
       <c r="D30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E30" t="n">
         <v>13</v>
@@ -82723,13 +82720,13 @@
         <v>343</v>
       </c>
       <c r="D31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E31" t="n">
         <v>0.5</v>
       </c>
       <c r="F31" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32">
@@ -82743,7 +82740,7 @@
         <v>343</v>
       </c>
       <c r="D32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E32" t="n">
         <v>0.04</v>
@@ -82763,7 +82760,7 @@
         <v>343</v>
       </c>
       <c r="D33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E33" t="n">
         <v>0.043</v>
@@ -82783,7 +82780,7 @@
         <v>343</v>
       </c>
       <c r="D34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E34" t="n">
         <v>0.0058</v>
@@ -82803,7 +82800,7 @@
         <v>343</v>
       </c>
       <c r="D35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E35" t="n">
         <v>6.6</v>
@@ -82823,7 +82820,7 @@
         <v>343</v>
       </c>
       <c r="D36" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E36" t="n">
         <v>15</v>
@@ -82843,7 +82840,7 @@
         <v>343</v>
       </c>
       <c r="D37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E37" t="n">
         <v>320</v>
@@ -82860,7 +82857,7 @@
         <v>120</v>
       </c>
       <c r="C38" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D38" t="s">
         <v>344</v>
@@ -82880,7 +82877,7 @@
         <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D39" t="s">
         <v>344</v>
@@ -82900,7 +82897,7 @@
         <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D40" t="s">
         <v>344</v>
@@ -82920,7 +82917,7 @@
         <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D41" t="s">
         <v>344</v>
@@ -82940,7 +82937,7 @@
         <v>133</v>
       </c>
       <c r="C42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D42" t="s">
         <v>344</v>
@@ -82960,7 +82957,7 @@
         <v>134</v>
       </c>
       <c r="C43" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D43" t="s">
         <v>344</v>
@@ -82980,7 +82977,7 @@
         <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D44" t="s">
         <v>344</v>
@@ -83000,7 +82997,7 @@
         <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D45" t="s">
         <v>344</v>
@@ -83020,7 +83017,7 @@
         <v>150</v>
       </c>
       <c r="C46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D46" t="s">
         <v>344</v>
@@ -83037,10 +83034,10 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C47" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D47" t="s">
         <v>344</v>
@@ -83060,7 +83057,7 @@
         <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D48" t="s">
         <v>344</v>
@@ -83069,7 +83066,7 @@
         <v>3.3</v>
       </c>
       <c r="F48" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49">
@@ -83080,7 +83077,7 @@
         <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D49" t="s">
         <v>344</v>
@@ -83100,7 +83097,7 @@
         <v>207</v>
       </c>
       <c r="C50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D50" t="s">
         <v>344</v>
@@ -83120,7 +83117,7 @@
         <v>209</v>
       </c>
       <c r="C51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D51" t="s">
         <v>344</v>
@@ -83140,10 +83137,10 @@
         <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D52" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E52" t="n">
         <v>0.86</v>
@@ -83160,10 +83157,10 @@
         <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E53" t="n">
         <v>0.012</v>
@@ -83180,10 +83177,10 @@
         <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D54" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E54" t="n">
         <v>0.015</v>
@@ -83200,10 +83197,10 @@
         <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E55" t="n">
         <v>0.04</v>
@@ -83220,10 +83217,10 @@
         <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D56" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E56" t="n">
         <v>1.1</v>
@@ -83240,10 +83237,10 @@
         <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E57" t="n">
         <v>0.4</v>
@@ -83260,10 +83257,10 @@
         <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E58" t="n">
         <v>0.025</v>
@@ -83280,10 +83277,10 @@
         <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D59" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E59" t="n">
         <v>110</v>
@@ -83300,10 +83297,10 @@
         <v>145</v>
       </c>
       <c r="C60" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D60" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E60" t="n">
         <v>2.1</v>
@@ -83320,10 +83317,10 @@
         <v>147</v>
       </c>
       <c r="C61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D61" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E61" t="n">
         <v>330</v>
@@ -83340,10 +83337,10 @@
         <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D62" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E62" t="n">
         <v>920</v>
@@ -83357,13 +83354,13 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C63" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D63" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E63" t="n">
         <v>45</v>
@@ -83380,10 +83377,10 @@
         <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D64" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E64" t="n">
         <v>1.8</v>
@@ -83400,10 +83397,10 @@
         <v>154</v>
       </c>
       <c r="C65" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D65" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E65" t="n">
         <v>5</v>
@@ -83420,10 +83417,10 @@
         <v>157</v>
       </c>
       <c r="C66" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D66" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E66" t="n">
         <v>7.8</v>
@@ -83440,16 +83437,16 @@
         <v>161</v>
       </c>
       <c r="C67" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E67" t="n">
         <v>0.2</v>
       </c>
       <c r="F67" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68">
@@ -83460,10 +83457,10 @@
         <v>164</v>
       </c>
       <c r="C68" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D68" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E68" t="n">
         <v>0.002</v>
@@ -83480,10 +83477,10 @@
         <v>178</v>
       </c>
       <c r="C69" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -83500,10 +83497,10 @@
         <v>207</v>
       </c>
       <c r="C70" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D70" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E70" t="n">
         <v>9.4</v>
@@ -83520,10 +83517,10 @@
         <v>209</v>
       </c>
       <c r="C71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E71" t="n">
         <v>320</v>

</xml_diff>

<commit_message>
Fixed a broken link
</commit_message>
<xml_diff>
--- a/vignettes/OWC_custom_bench.xlsx
+++ b/vignettes/OWC_custom_bench.xlsx
@@ -1069,7 +1069,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1107,7 +1107,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>